<commit_message>
fix: :bug: shift inputs when input is empty
</commit_message>
<xml_diff>
--- a/data/斷字比對(00000).xlsx
+++ b/data/斷字比對(00000).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eddie\Project\Python\icd-tokenize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5C1A18-01E3-4B9E-A6D6-443744350593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E30837-0D8F-4E7F-87B6-C4D6C8BD6939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -458,6 +458,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1296,19 +1299,19 @@
   <dimension ref="A1:AT10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="AT1" sqref="AT1:AT1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="21" width="9.140625" style="11"/>
     <col min="22" max="23" width="9.140625" style="12"/>
-    <col min="24" max="44" width="9.140625" style="11"/>
-    <col min="45" max="45" width="11.140625" style="11" customWidth="1"/>
-    <col min="46" max="46" width="11.140625" style="12" customWidth="1"/>
+    <col min="24" max="43" width="9.140625" style="11"/>
+    <col min="44" max="44" width="9.140625" style="12"/>
+    <col min="45" max="46" width="11.140625" style="12" customWidth="1"/>
     <col min="47" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
@@ -1325,6 +1328,7 @@
       </c>
       <c r="Y1" s="6"/>
       <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
     </row>
     <row r="2" spans="1:46" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1597,10 +1601,10 @@
       <c r="AQ3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AR3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AR3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS3" s="12" t="s">
         <v>28</v>
       </c>
       <c r="AT3" s="12" t="s">
@@ -1674,7 +1678,7 @@
       <c r="AR4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS4" s="10" t="b">
+      <c r="AS4" s="8" t="b">
         <f>EXACT(W4,AR4)</f>
         <v>1</v>
       </c>
@@ -1710,13 +1714,13 @@
       <c r="AD5" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="AR5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT5" s="11" t="s">
+      <c r="AR5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT5" s="12" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1795,7 +1799,7 @@
       <c r="AR6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS6" s="10" t="b">
+      <c r="AS6" s="8" t="b">
         <f t="shared" ref="AS6:AS10" si="0">EXACT(W6,AR6)</f>
         <v>1</v>
       </c>
@@ -1872,7 +1876,7 @@
       <c r="AR7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS7" s="10" t="b">
+      <c r="AS7" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1947,7 +1951,7 @@
       <c r="AR8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS8" s="10" t="b">
+      <c r="AS8" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2016,7 +2020,7 @@
       <c r="AR9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS9" s="10" t="b">
+      <c r="AS9" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2085,7 +2089,7 @@
       <c r="AR10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AS10" s="10" t="b">
+      <c r="AS10" s="8" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
feat: :construction: shift input when encounter special word
</commit_message>
<xml_diff>
--- a/data/斷字比對(00000).xlsx
+++ b/data/斷字比對(00000).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eddie\Project\Python\icd-tokenize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E30837-0D8F-4E7F-87B6-C4D6C8BD6939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C8B135-CA9F-4B34-8677-E120337648E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="83">
   <si>
     <t>NO</t>
   </si>
@@ -345,6 +345,33 @@
   </si>
   <si>
     <t>035285</t>
+  </si>
+  <si>
+    <t>跌倒致頸椎骨折。</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>頸椎骨折</t>
+  </si>
+  <si>
+    <t>跌倒</t>
+  </si>
+  <si>
+    <t>030654</t>
+  </si>
+  <si>
+    <t>嗆咳導致肺炎合併呼吸衰竭</t>
+  </si>
+  <si>
+    <t>呼吸衰竭</t>
+  </si>
+  <si>
+    <t>嗆咳</t>
+  </si>
+  <si>
+    <t>100472</t>
   </si>
 </sst>
 </file>
@@ -1296,13 +1323,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT10"/>
+  <dimension ref="A1:AT12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT1" sqref="AT1:AT1048576"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2097,6 +2124,175 @@
         <v>70</v>
       </c>
     </row>
+    <row r="11" spans="1:46" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="V11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="W11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="X11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT11" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT12" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AT3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat: :sparkles: add validation for combination
</commit_message>
<xml_diff>
--- a/data/斷字比對(00000).xlsx
+++ b/data/斷字比對(00000).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eddie\Project\Python\icd-tokenize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E30837-0D8F-4E7F-87B6-C4D6C8BD6939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C066A34F-65F1-4C68-BA07-E749E9F95577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
   <si>
     <t>NO</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>035285</t>
+  </si>
+  <si>
+    <t>高血壓心臟病</t>
+  </si>
+  <si>
+    <t>陳舊性腦梗塞</t>
+  </si>
+  <si>
+    <t>010935</t>
   </si>
 </sst>
 </file>
@@ -1296,13 +1305,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT10"/>
+  <dimension ref="A1:AT11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AT1" sqref="AT1:AT1048576"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,7 +1809,7 @@
         <v>28</v>
       </c>
       <c r="AS6" s="8" t="b">
-        <f t="shared" ref="AS6:AS10" si="0">EXACT(W6,AR6)</f>
+        <f t="shared" ref="AS6:AS11" si="0">EXACT(W6,AR6)</f>
         <v>1</v>
       </c>
       <c r="AT6" s="8" t="s">
@@ -2097,6 +2106,75 @@
         <v>70</v>
       </c>
     </row>
+    <row r="11" spans="1:46" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS11" s="10" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AT11" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:AT3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>